<commit_message>
sim of g_face xlsx
</commit_message>
<xml_diff>
--- a/similarity-G_face.xlsx
+++ b/similarity-G_face.xlsx
@@ -348,7 +348,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -359,39 +359,36 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>9629</v>
+        <v>9591</v>
       </c>
       <c r="C1">
-        <v>-5.101501585878374</v>
+        <v>-5.093656146319681</v>
       </c>
       <c r="D1">
-        <v>0.01570666537433818</v>
+        <v>0.0193415503636275</v>
       </c>
       <c r="E1">
-        <v>-0.5129077872972849</v>
+        <v>-0.5473360161963243</v>
       </c>
       <c r="F1">
-        <v>-0.0002370561611335486</v>
+        <v>-0.000243596229282723</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
       <c r="B2">
-        <v>0.1091302672439196</v>
+        <v>0.1086995942607158</v>
       </c>
       <c r="C2">
-        <v>-0.1167631803237004</v>
+        <v>-0.1165836138845864</v>
       </c>
       <c r="D2">
-        <v>0.02593799106059122</v>
+        <v>0.03194064102552283</v>
       </c>
       <c r="E2">
-        <v>-0.1389050334028379</v>
+        <v>-0.1482288424844297</v>
       </c>
       <c r="F2">
-        <v>-0.3554292619920535</v>
+        <v>-0.3652350885292057</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -399,24 +396,36 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>10412</v>
+        <v>10380</v>
       </c>
       <c r="C3">
-        <v>-4.792747642660707</v>
+        <v>-4.790026433593951</v>
+      </c>
+      <c r="D3">
+        <v>0.004338641393008991</v>
+      </c>
+      <c r="E3">
+        <v>-0.4704605560049546</v>
+      </c>
+      <c r="F3">
+        <v>-0.0002285109690096757</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
       <c r="B4">
-        <v>0.1180043973978285</v>
+        <v>0.1176417254119727</v>
       </c>
       <c r="C4">
-        <v>-0.1096964193434878</v>
+        <v>-0.109634136303953</v>
       </c>
       <c r="D4">
-        <v>0.002245575127464039</v>
+        <v>0.007164833463049446</v>
+      </c>
+      <c r="E4">
+        <v>-0.1274095283110002</v>
+      </c>
+      <c r="F4">
+        <v>-0.3426170603785406</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -424,33 +433,36 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>9656</v>
+        <v>9610</v>
       </c>
       <c r="C5">
-        <v>-5.090854898181213</v>
+        <v>-5.086159598677149</v>
       </c>
       <c r="D5">
-        <v>0.003708343317558103</v>
+        <v>0.01077887566893254</v>
       </c>
       <c r="E5">
-        <v>-0.4262027993874344</v>
+        <v>-0.5344295944299597</v>
+      </c>
+      <c r="F5">
+        <v>-0.0002410490767730831</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
       <c r="B6">
-        <v>0.1094362717319854</v>
+        <v>0.1089149307523177</v>
       </c>
       <c r="C6">
-        <v>-0.1165194989105896</v>
+        <v>-0.116412032884472</v>
+      </c>
+      <c r="D6">
+        <v>0.01780023792961064</v>
       </c>
       <c r="E6">
-        <v>-0.1154236990575869</v>
+        <v>-0.1447335417871742</v>
       </c>
       <c r="F6">
-        <v>-0.0002199545856089238</v>
+        <v>-0.3614160250112891</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -458,30 +470,36 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>13859</v>
+        <v>13756</v>
       </c>
       <c r="C7">
-        <v>-1.223042576971032</v>
+        <v>-1.248232768377648</v>
       </c>
       <c r="D7">
-        <v>0.006814865652124191</v>
+        <v>0.006010726913679099</v>
+      </c>
+      <c r="E7">
+        <v>-0.9491832293345732</v>
       </c>
       <c r="F7">
-        <v>-0.3297880791662065</v>
+        <v>-0.0003040673443081121</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
       <c r="B8">
-        <v>0.1570709703742321</v>
+        <v>0.1559036199197588</v>
       </c>
       <c r="C8">
-        <v>-0.02799300138487431</v>
+        <v>-0.02856955454517147</v>
       </c>
       <c r="D8">
-        <v>0.01125407081332027</v>
+        <v>0.009926115902958353</v>
+      </c>
+      <c r="E8">
+        <v>-0.2570565927081809</v>
+      </c>
+      <c r="F8">
+        <v>-0.4559022269935047</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -489,238 +507,184 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>12796</v>
+        <v>12755</v>
       </c>
       <c r="C9">
-        <v>-1.682696618571832</v>
+        <v>-1.69101262688784</v>
+      </c>
+      <c r="D9">
+        <v>0.0007338155379026379</v>
       </c>
       <c r="E9">
-        <v>-0.4953388124810014</v>
+        <v>-0.8742960386443186</v>
+      </c>
+      <c r="F9">
+        <v>-0.0002887150412807448</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10">
-        <v>0.1450234603440851</v>
+        <v>0.1445587868622073</v>
       </c>
       <c r="C10">
-        <v>-0.0385135641726071</v>
+        <v>-0.03870390099054778</v>
       </c>
       <c r="D10">
-        <v>-0.01059493417763635</v>
+        <v>0.001211823159697484</v>
       </c>
       <c r="E10">
-        <v>-0.1341470260296821</v>
+        <v>-0.2367757391475674</v>
+      </c>
+      <c r="F10">
+        <v>-0.4328838092953397</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
       <c r="B11">
-        <v>13776</v>
+        <v>13660</v>
       </c>
       <c r="C11">
-        <v>-1.231075061851421</v>
+        <v>-1.208627803039604</v>
       </c>
       <c r="D11">
-        <v>-0.01749647690566296</v>
+        <v>0.01856820234004986</v>
+      </c>
+      <c r="E11">
+        <v>-0.9210961664486081</v>
       </c>
       <c r="F11">
-        <v>-0.000233590880104694</v>
+        <v>-0.0002975286429527335</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12">
-        <v>0.1561302899109187</v>
+        <v>0.1548156039621914</v>
       </c>
       <c r="C12">
-        <v>-0.02817684891775216</v>
+        <v>-0.02766307600515086</v>
+      </c>
+      <c r="D12">
+        <v>0.03066353390926277</v>
+      </c>
+      <c r="E12">
+        <v>-0.249450090126263</v>
       </c>
       <c r="F12">
-        <v>-0.3502336059382672</v>
+        <v>-0.4460984497534803</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
       <c r="B13">
-        <v>21893</v>
+        <v>21670</v>
       </c>
       <c r="C13">
-        <v>2.04279135982312</v>
+        <v>2.092782415811598</v>
       </c>
       <c r="D13">
-        <v>-0.01078221094863585</v>
+        <v>-0.00559351700145394</v>
       </c>
       <c r="E13">
-        <v>-0.9292257292283552</v>
+        <v>-0.9280221937219415</v>
+      </c>
+      <c r="F13">
+        <v>-0.0002992797873846994</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14">
-        <v>0.2481243058231521</v>
+        <v>0.2455969354217195</v>
       </c>
       <c r="C14">
-        <v>0.04675541345924237</v>
+        <v>0.04789960886655397</v>
       </c>
       <c r="D14">
-        <v>-0.01780574581133264</v>
+        <v>-0.00923713535134065</v>
       </c>
       <c r="E14">
-        <v>-0.2516517279594915</v>
+        <v>-0.2513257880072033</v>
+      </c>
+      <c r="F14">
+        <v>-0.4487240215594141</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
       <c r="B15">
-        <v>20760</v>
+        <v>20521</v>
       </c>
       <c r="C15">
-        <v>1.497212912083967</v>
+        <v>1.519962222415842</v>
+      </c>
+      <c r="D15">
+        <v>-0.005438136747905942</v>
+      </c>
+      <c r="E15">
+        <v>-0.9241710323063232</v>
+      </c>
+      <c r="F15">
+        <v>-0.0002992435250181504</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16">
-        <v>0.2352834508239454</v>
+        <v>0.232574744429585</v>
       </c>
       <c r="C16">
-        <v>0.0342682126612595</v>
+        <v>0.03478889892976395</v>
       </c>
       <c r="D16">
-        <v>-0.01048830098645848</v>
+        <v>-0.008980540362431988</v>
+      </c>
+      <c r="E16">
+        <v>-0.2502828213798199</v>
       </c>
       <c r="F16">
-        <v>-0.0003000657379658156</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+        <v>-0.4486696517167617</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
       <c r="B17">
-        <v>20526</v>
+        <v>20293</v>
       </c>
       <c r="C17">
-        <v>1.446982807849658</v>
+        <v>1.49091909667586</v>
       </c>
       <c r="D17">
-        <v>-0.01732038282753656</v>
+        <v>-0.0044813020838812</v>
       </c>
       <c r="E17">
-        <v>-0.8750588820300829</v>
+        <v>-0.9228827440297103</v>
       </c>
       <c r="F17">
-        <v>-0.4499024336018287</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+        <v>-0.0002984392174172367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="B18">
-        <v>0.2326314119273749</v>
+        <v>0.2299907065303624</v>
       </c>
       <c r="C18">
-        <v>0.0331185459171338</v>
+        <v>0.03412415979936192</v>
+      </c>
+      <c r="D18">
+        <v>-0.007400423363028267</v>
       </c>
       <c r="E18">
-        <v>-0.2369823314212763</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="D19">
-        <v>-0.02055169458517292</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="D20">
-        <v>-0.03393907349049115</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="E21">
-        <v>-0.9140343488927773</v>
-      </c>
-      <c r="F21">
-        <v>-0.0002889523719174676</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="D22">
-        <v>-0.03091750769435719</v>
-      </c>
-      <c r="E22">
-        <v>-0.2475376176940422</v>
-      </c>
-      <c r="F22">
-        <v>-0.4332396500912724</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="D23">
-        <v>-0.05105717980738403</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="D25">
-        <v>-0.02992146790401418</v>
-      </c>
-      <c r="E25">
-        <v>-0.8978718842126971</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="D26">
-        <v>-0.04941231945273991</v>
-      </c>
-      <c r="E26">
-        <v>-0.2431605196037816</v>
-      </c>
-      <c r="F26">
-        <v>-0.0002966736798370808</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="F27">
-        <v>-0.4448165640274406</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="E29">
-        <v>-0.8880987120722583</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="E30">
-        <v>-0.2405137615777965</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="F31">
-        <v>-0.0002941623910475759</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="F32">
-        <v>-0.4410512726431774</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
-      <c r="E33">
-        <v>-0.8952927813694052</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
-      <c r="E34">
-        <v>-0.2424620502580838</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
-      <c r="F36">
-        <v>-0.0002927540931600112</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
-      <c r="F37">
-        <v>-0.4389397465117807</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6">
-      <c r="F41">
-        <v>-0.0002938591487918501</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
-      <c r="F42">
-        <v>-0.440596607509641</v>
+        <v>-0.2499339287902993</v>
+      </c>
+      <c r="F18">
+        <v>-0.4474637161458811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>